<commit_message>
Added Notes Checked Question QID Creation
</commit_message>
<xml_diff>
--- a/AutomationTest.xlsx
+++ b/AutomationTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-1485" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="29490" yWindow="2475" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -41,8 +41,21 @@
       <sz val="12"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -55,6 +68,31 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF4229"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF29FF49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF4229"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0029FF49"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF4229"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -65,10 +103,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
@@ -89,13 +128,26 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -472,21 +524,21 @@
   </sheetPr>
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:N4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="18" customWidth="1" style="8" min="1" max="1"/>
-    <col width="18.140625" customWidth="1" style="8" min="2" max="2"/>
+    <col width="18" customWidth="1" style="12" min="1" max="1"/>
+    <col width="18.140625" customWidth="1" style="12" min="2" max="2"/>
     <col width="9.140625" customWidth="1" style="1" min="3" max="3"/>
-    <col width="13.7109375" customWidth="1" style="8" min="4" max="4"/>
-    <col width="22.28515625" customWidth="1" style="8" min="5" max="5"/>
-    <col width="15.140625" customWidth="1" style="8" min="6" max="6"/>
-    <col width="21.7109375" customWidth="1" style="8" min="8" max="8"/>
-    <col width="10.85546875" customWidth="1" style="8" min="9" max="9"/>
-    <col width="44.42578125" customWidth="1" style="8" min="10" max="10"/>
+    <col width="21" customWidth="1" style="12" min="4" max="4"/>
+    <col width="22.28515625" customWidth="1" style="12" min="5" max="5"/>
+    <col width="32.140625" customWidth="1" style="12" min="6" max="6"/>
+    <col width="21.7109375" customWidth="1" style="12" min="8" max="8"/>
+    <col width="10.85546875" customWidth="1" style="12" min="9" max="9"/>
+    <col width="44.42578125" customWidth="1" style="12" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -580,8 +632,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="105" customFormat="1" customHeight="1" s="6">
-      <c r="A4" s="4" t="n"/>
+    <row r="4" ht="60" customHeight="1" s="12">
       <c r="B4" s="4" t="inlineStr">
         <is>
           <t>Dummy Question</t>
@@ -589,7 +640,7 @@
       </c>
       <c r="C4" s="4" t="inlineStr">
         <is>
-          <t>Application</t>
+          <t>Multiple Choice</t>
         </is>
       </c>
       <c r="D4" s="4" t="inlineStr">
@@ -607,8 +658,7 @@
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t>example
-Examples</t>
+          <t>A: example</t>
         </is>
       </c>
       <c r="G4" s="4" t="inlineStr">
@@ -621,27 +671,32 @@
           <t>This is the explanation/helptext</t>
         </is>
       </c>
+      <c r="I4" s="6" t="n"/>
       <c r="J4" s="7" t="inlineStr">
         <is>
           <t>Apply different views to a document
 test to check if it is broke test</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>400146</t>
+      <c r="K4" s="6" t="n"/>
+      <c r="L4" s="6" t="n"/>
+      <c r="M4" s="6" t="n"/>
+      <c r="N4" s="16" t="inlineStr">
+        <is>
+          <t>411782</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="60" customHeight="1" s="8">
+    <row r="5" ht="228.75" customHeight="1" s="12">
+      <c r="A5" s="4" t="n"/>
       <c r="B5" s="4" t="inlineStr">
         <is>
           <t>Dummy Question</t>
         </is>
       </c>
-      <c r="C5" s="4" t="inlineStr">
-        <is>
-          <t>Multiple Choice</t>
+      <c r="C5" s="8" t="inlineStr">
+        <is>
+          <t>Short Answer</t>
         </is>
       </c>
       <c r="D5" s="4" t="inlineStr">
@@ -659,8 +714,7 @@
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t>example
-Examples</t>
+          <t>A: example</t>
         </is>
       </c>
       <c r="G5" s="4" t="inlineStr">
@@ -683,26 +737,39 @@
       <c r="K5" s="6" t="n"/>
       <c r="L5" s="6" t="n"/>
       <c r="M5" s="6" t="n"/>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>400145</t>
+      <c r="N5" s="17" t="inlineStr">
+        <is>
+          <t>411783</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="60" customHeight="1" s="8">
+    <row r="6" ht="102.75" customHeight="1" s="12">
       <c r="B6" s="4" t="inlineStr">
         <is>
           <t>Dummy Question</t>
         </is>
       </c>
-      <c r="C6" s="1" t="inlineStr">
-        <is>
-          <t>IFrame</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>Do the Question This way. Instructions</t>
+      <c r="C6" s="8" t="inlineStr">
+        <is>
+          <t>Single True False</t>
+        </is>
+      </c>
+      <c r="D6" s="8" t="inlineStr">
+        <is>
+          <t>Drag and drop the correct project terms to their definitions.</t>
+        </is>
+      </c>
+      <c r="F6" s="8" t="inlineStr">
+        <is>
+          <t>Step 1: Drag Iteration to A cycle of a design plan
+Step 2: Drag Change orders to Formal changes to the project scope
+Step 3: Drag Feedback loop to The order in which feedback is presented on an aspect of a project
+Step 4: Drag Scope creep to The act of unauthorized change to a project scope</t>
+        </is>
+      </c>
+      <c r="G6" s="4" t="inlineStr">
+        <is>
+          <t>This is the Hint.</t>
         </is>
       </c>
       <c r="H6" s="5" t="inlineStr">
@@ -710,10 +777,15 @@
           <t>This is the explanation/helptext</t>
         </is>
       </c>
-      <c r="J6" s="9" t="inlineStr">
+      <c r="J6" s="7" t="inlineStr">
         <is>
           <t>Apply different views to a document
 test to check if it is broke test</t>
+        </is>
+      </c>
+      <c r="N6" s="17" t="inlineStr">
+        <is>
+          <t>411784</t>
         </is>
       </c>
     </row>
@@ -731,13 +803,13 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="30" customHeight="1" s="8">
+    <row r="1" ht="30" customHeight="1" s="12">
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="1" t="inlineStr">
         <is>
@@ -760,7 +832,7 @@
       <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="n"/>
     </row>
-    <row r="2" ht="45" customHeight="1" s="8">
+    <row r="2" ht="45" customHeight="1" s="12">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="inlineStr">
         <is>
@@ -775,7 +847,7 @@
       <c r="H2" s="1" t="n"/>
       <c r="I2" s="1" t="n"/>
     </row>
-    <row r="3" ht="30" customHeight="1" s="8">
+    <row r="3" ht="30" customHeight="1" s="12">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>ID</t>
@@ -829,7 +901,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="173.25" customHeight="1" s="8">
+    <row r="4" ht="173.25" customHeight="1" s="12">
       <c r="A4" s="4" t="n"/>
       <c r="B4" s="4" t="inlineStr">
         <is>
@@ -882,12 +954,13 @@
       <c r="M4" s="6" t="n"/>
       <c r="N4" t="inlineStr">
         <is>
-          <t>400147</t>
+          <t>411737</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360"/>
 </worksheet>
 </file>
 
@@ -897,14 +970,59 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A3:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" ht="362.25" customHeight="1" s="12">
+      <c r="A3" s="10" t="inlineStr">
+        <is>
+          <t>Open Panels</t>
+        </is>
+      </c>
+      <c r="B3" s="10" t="inlineStr">
+        <is>
+          <t>T/F</t>
+        </is>
+      </c>
+      <c r="C3" s="11" t="inlineStr">
+        <is>
+          <t>Once a panel is open, it cannot be rearranged within the workspace.</t>
+        </is>
+      </c>
+      <c r="D3" s="9" t="n"/>
+      <c r="E3" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11" t="inlineStr">
+        <is>
+          <t>Panels can be collapsed down to icons</t>
+        </is>
+      </c>
+      <c r="G3" s="11" t="inlineStr">
+        <is>
+          <t>Once a panel is open, it can be rearranged within the workspace at any point in time.</t>
+        </is>
+      </c>
+      <c r="H3" s="11" t="inlineStr">
+        <is>
+          <t>Application Workspace
+   Workspace Organization and Customization</t>
+        </is>
+      </c>
+      <c r="I3" s="11" t="inlineStr">
+        <is>
+          <t>2 Project Setup and Interface
+2.2 Navigate, organize, and customize the application workspace
+2.2.b Organize and customize the workspace</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wrap the QIDCELL when Error Handling
</commit_message>
<xml_diff>
--- a/AutomationTest.xlsx
+++ b/AutomationTest.xlsx
@@ -97,7 +97,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
@@ -133,6 +133,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,7 +675,7 @@
       <c r="M4" s="6" t="n"/>
       <c r="N4" s="14" t="inlineStr">
         <is>
-          <t>412046</t>
+          <t>412051</t>
         </is>
       </c>
     </row>
@@ -722,9 +725,9 @@
       <c r="K5" s="6" t="n"/>
       <c r="L5" s="6" t="n"/>
       <c r="M5" s="6" t="n"/>
-      <c r="N5" s="15" t="inlineStr">
-        <is>
-          <t>Question Failed To Create</t>
+      <c r="N5" s="17" t="inlineStr">
+        <is>
+          <t>Question Failed To Create:Object failed to Match any listed under this product</t>
         </is>
       </c>
     </row>
@@ -770,7 +773,7 @@
       </c>
       <c r="N6" s="16" t="inlineStr">
         <is>
-          <t>412047</t>
+          <t>412050</t>
         </is>
       </c>
     </row>

</xml_diff>